<commit_message>
tambah halaman daily visit dan timestamp
</commit_message>
<xml_diff>
--- a/Book 1.xlsx
+++ b/Book 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\slm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D0A0DC-021F-4529-A01A-291CCF25B039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2D085A-9536-4FD2-9F7C-9B90B65E3F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Customer" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Daily Visit'!$A$1:$J$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Customer'!$A$1:$C$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Customer'!$A$10:$K$390</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PO!$A$1:$N$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Stock!$A$1:$I$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Timestamp!$A$1:$N$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Timestamp!$A$1:$M$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3919" uniqueCount="1726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3918" uniqueCount="1726">
   <si>
     <t>CLASS</t>
   </si>
@@ -5263,7 +5263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -5299,11 +5299,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5340,6 +5355,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5677,8 +5704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J390" sqref="J390"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17983,7 +18010,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C8" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A10:K390" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17998,158 +18025,158 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>1695</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>1696</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="13" t="s">
         <v>1697</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>1698</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15" t="s">
         <v>1699</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="15" t="s">
         <v>1700</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
         <v>1701</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="15" t="s">
         <v>1702</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15" t="s">
         <v>1703</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="15" t="s">
         <v>1704</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>1705</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="15" t="s">
         <v>1706</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>1707</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="15" t="s">
         <v>1708</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>1707</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="15" t="s">
         <v>1709</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J7" xr:uid="{FDB8E0F9-65FC-4893-8F01-92626997472E}"/>
@@ -18159,221 +18186,211 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263E2F35-84B1-4434-827A-C6D4A67EAA42}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="15.28515625" style="2"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="15.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1695</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1696</v>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>23</v>
+        <v>1697</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1697</v>
+        <v>1710</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>1712</v>
+        <v>1698</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>1698</v>
-      </c>
-      <c r="N1" s="3" t="s">
         <v>1713</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>1699</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1700</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>1714</v>
       </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>1701</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>1715</v>
       </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>1703</v>
+      </c>
       <c r="H4" s="1" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1704</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>1715</v>
       </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>1705</v>
+      </c>
       <c r="H5" s="1" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1706</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>1715</v>
       </c>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>1707</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1708</v>
-      </c>
-      <c r="J6" s="1" t="s">
         <v>1715</v>
       </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>1707</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>1707</v>
+        <v>1709</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1709</v>
-      </c>
-      <c r="J7" s="1" t="s">
         <v>1715</v>
       </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N7" xr:uid="{263E2F35-84B1-4434-827A-C6D4A67EAA42}"/>
+  <autoFilter ref="A1:M7" xr:uid="{263E2F35-84B1-4434-827A-C6D4A67EAA42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18388,18 +18405,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="15.140625" style="2"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="15.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -18573,17 +18596,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781D5132-FCA4-4BC4-9142-52B9CF7A75DF}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tambah halaman purchase order
</commit_message>
<xml_diff>
--- a/Book 1.xlsx
+++ b/Book 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\slm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2D085A-9536-4FD2-9F7C-9B90B65E3F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F7AB47-596D-4C32-B0CE-356BB633494D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5705,7 +5705,7 @@
   <dimension ref="A1:K390"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12691,7 +12691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:11" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A225" s="10" t="s">
         <v>988</v>
       </c>
@@ -12886,7 +12886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" spans="1:11" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" s="10" t="s">
         <v>1005</v>
       </c>

</xml_diff>

<commit_message>
tambah halaman daftar stock card
</commit_message>
<xml_diff>
--- a/Book 1.xlsx
+++ b/Book 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\slm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F7AB47-596D-4C32-B0CE-356BB633494D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878A9278-C335-498E-9A53-7BB33B05A3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Customer" sheetId="1" r:id="rId1"/>
@@ -5704,8 +5704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K390"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18596,7 +18596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781D5132-FCA4-4BC4-9142-52B9CF7A75DF}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>